<commit_message>
Reports rafael week 9
Reports rafael week 9
</commit_message>
<xml_diff>
--- a/NoteBook/task and schedule plans and actual/SCHEDULE_Rafael_Ortega_ciclo2.xlsx
+++ b/NoteBook/task and schedule plans and actual/SCHEDULE_Rafael_Ortega_ciclo2.xlsx
@@ -119,7 +119,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -272,26 +272,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -312,8 +297,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -325,6 +319,78 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -332,93 +398,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -724,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15:K15"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,14 +720,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -771,213 +750,213 @@
       <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="36" t="s">
+      <c r="B3" s="15"/>
+      <c r="C3" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="12" t="s">
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="12"/>
-      <c r="J3" s="13">
+      <c r="I3" s="39"/>
+      <c r="J3" s="40">
         <v>41752</v>
       </c>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
     </row>
     <row r="4" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="37" t="s">
+      <c r="B4" s="15"/>
+      <c r="C4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="12" t="s">
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="12"/>
-      <c r="J4" s="15" t="s">
+      <c r="I4" s="39"/>
+      <c r="J4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
     </row>
     <row r="5" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="37">
+      <c r="B5" s="15"/>
+      <c r="C5" s="17">
         <v>1</v>
       </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="12" t="s">
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="12"/>
-      <c r="J5" s="15">
+      <c r="I5" s="39"/>
+      <c r="J5" s="24">
         <v>2</v>
       </c>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="38"/>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
-      <c r="B7" s="39"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="40" t="s">
+      <c r="B7" s="19"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="41"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="40" t="s">
+      <c r="E7" s="22"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="42"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="23"/>
     </row>
     <row r="8" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="9" t="s">
+      <c r="C8" s="35"/>
+      <c r="D8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="20"/>
-      <c r="I8" s="9" t="s">
+      <c r="H8" s="29"/>
+      <c r="I8" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="19" t="s">
+      <c r="J8" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="K8" s="20"/>
-      <c r="L8" s="9" t="s">
+      <c r="K8" s="29"/>
+      <c r="L8" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="10"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="13"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="10"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="13"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="33"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="10"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="13"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="33"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="10"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="13"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="34"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="24"/>
-      <c r="L13" s="11"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="14"/>
     </row>
     <row r="14" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>6</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="17"/>
+      <c r="C14" s="26"/>
       <c r="D14" s="6">
         <v>1.3</v>
       </c>
@@ -986,21 +965,20 @@
         <v>1.3</v>
       </c>
       <c r="F14" s="7">
-        <f>ROUND((D14/D18)*100,1)</f>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="G14" s="18">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="G14" s="25">
         <v>0</v>
       </c>
-      <c r="H14" s="17"/>
+      <c r="H14" s="26"/>
       <c r="I14" s="6">
         <f>G14</f>
         <v>0</v>
       </c>
-      <c r="J14" s="18">
+      <c r="J14" s="25">
         <v>0</v>
       </c>
-      <c r="K14" s="17"/>
+      <c r="K14" s="26"/>
       <c r="L14" s="6">
         <f>J14</f>
         <v>0</v>
@@ -1010,10 +988,10 @@
       <c r="A15" s="5">
         <v>7</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="27">
         <v>41752</v>
       </c>
-      <c r="C15" s="17"/>
+      <c r="C15" s="26"/>
       <c r="D15" s="7">
         <v>7</v>
       </c>
@@ -1022,34 +1000,33 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="F15" s="7">
-        <f>ROUND((D15/D18)*100,1)</f>
-        <v>23.9</v>
-      </c>
-      <c r="G15" s="18">
+        <v>28.33</v>
+      </c>
+      <c r="G15" s="25">
         <v>10.5</v>
       </c>
-      <c r="H15" s="17"/>
+      <c r="H15" s="26"/>
       <c r="I15" s="7">
         <f>G15+I14</f>
         <v>10.5</v>
       </c>
-      <c r="J15" s="18">
-        <v>28.2</v>
-      </c>
-      <c r="K15" s="17"/>
+      <c r="J15" s="25">
+        <v>28.33</v>
+      </c>
+      <c r="K15" s="26"/>
       <c r="L15" s="7">
         <f>J15+L14</f>
-        <v>28.2</v>
+        <v>28.33</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>8</v>
       </c>
-      <c r="B16" s="16">
+      <c r="B16" s="27">
         <v>41759</v>
       </c>
-      <c r="C16" s="17"/>
+      <c r="C16" s="26"/>
       <c r="D16" s="7">
         <v>12.5</v>
       </c>
@@ -1058,33 +1035,33 @@
         <v>20.8</v>
       </c>
       <c r="F16" s="7">
-        <f>ROUND((D16/D18)*100,1)</f>
-        <v>42.7</v>
-      </c>
-      <c r="G16" s="18">
+        <v>70.989999999999995</v>
+      </c>
+      <c r="G16" s="25">
         <v>16.3</v>
       </c>
-      <c r="H16" s="17"/>
+      <c r="H16" s="26"/>
       <c r="I16" s="7">
         <f>G16+I15</f>
         <v>26.8</v>
       </c>
-      <c r="J16" s="18">
-        <v>42.5</v>
-      </c>
-      <c r="K16" s="17"/>
+      <c r="J16" s="25">
+        <v>42.66</v>
+      </c>
+      <c r="K16" s="26"/>
       <c r="L16" s="7">
-        <v>70.7</v>
+        <f t="shared" ref="L16:L17" si="1">J16+L15</f>
+        <v>70.989999999999995</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>9</v>
       </c>
-      <c r="B17" s="16">
+      <c r="B17" s="27">
         <v>41766</v>
       </c>
-      <c r="C17" s="17"/>
+      <c r="C17" s="26"/>
       <c r="D17" s="7">
         <v>8.5</v>
       </c>
@@ -1093,38 +1070,48 @@
         <v>29.3</v>
       </c>
       <c r="F17" s="7">
-        <f>ROUND((D17/D18)*100,1)</f>
-        <v>29</v>
-      </c>
-      <c r="G17" s="18"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="7"/>
-    </row>
-    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="43"/>
-      <c r="B18" s="43"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="8">
-        <f>SUM(D14:D17)</f>
-        <v>29.3</v>
-      </c>
-      <c r="E18" s="43"/>
-      <c r="F18" s="8">
-        <f>SUM(F14:F17)</f>
         <v>100</v>
       </c>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="43"/>
-      <c r="L18" s="43"/>
+      <c r="G17" s="25">
+        <v>11.6</v>
+      </c>
+      <c r="H17" s="26"/>
+      <c r="I17" s="7">
+        <v>38.4</v>
+      </c>
+      <c r="J17" s="25">
+        <v>29.01</v>
+      </c>
+      <c r="K17" s="26"/>
+      <c r="L17" s="7">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="L8:L13"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J8:K13"/>
+    <mergeCell ref="B8:C13"/>
+    <mergeCell ref="G8:H13"/>
+    <mergeCell ref="I8:I13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="G14:H14"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A8:A13"/>
     <mergeCell ref="D8:D13"/>
@@ -1141,28 +1128,6 @@
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="G7:L7"/>
     <mergeCell ref="J5:L5"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J8:K13"/>
-    <mergeCell ref="B8:C13"/>
-    <mergeCell ref="G8:H13"/>
-    <mergeCell ref="I8:I13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="L8:L13"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="J4:L4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>